<commit_message>
Table TypeBesoin et todo vao2
</commit_message>
<xml_diff>
--- a/todo/FinalWeb.xlsx
+++ b/todo/FinalWeb.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
   <si>
     <t xml:space="preserve">Tâches </t>
   </si>
@@ -52,6 +52,9 @@
     <t>Christian</t>
   </si>
   <si>
+    <t>FIni</t>
+  </si>
+  <si>
     <t>id_besoin</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
     <t>equivalence_besoin</t>
   </si>
   <si>
+    <t>Fini</t>
+  </si>
+  <si>
     <t>id_equivalence_besoin</t>
   </si>
   <si>
@@ -100,10 +106,10 @@
     <t>id_don</t>
   </si>
   <si>
-    <t>date_don</t>
-  </si>
-  <si>
-    <t>point_total</t>
+    <t>date</t>
+  </si>
+  <si>
+    <t>prix_total</t>
   </si>
   <si>
     <t>donnation</t>
@@ -112,6 +118,12 @@
     <t>id_donnation</t>
   </si>
   <si>
+    <t>dispatch</t>
+  </si>
+  <si>
+    <t>date_dispatch</t>
+  </si>
+  <si>
     <t>Modèles</t>
   </si>
   <si>
@@ -176,12 +188,6 @@
   </si>
   <si>
     <t>Collaborateurs</t>
-  </si>
-  <si>
-    <t>Fini</t>
-  </si>
-  <si>
-    <t>FIni</t>
   </si>
 </sst>
 </file>
@@ -1120,10 +1126,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.8" outlineLevelCol="4"/>
@@ -1180,17 +1186,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="3:3">
@@ -1200,45 +1209,48 @@
     </row>
     <row r="9" spans="3:3">
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -1246,17 +1258,17 @@
     </row>
     <row r="17" spans="3:3">
       <c r="C17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -1264,102 +1276,96 @@
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="3:3">
       <c r="C25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3">
-      <c r="C27" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="3:3">
       <c r="C29" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="3:3">
       <c r="C30" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="3:3">
       <c r="C31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" t="s">
         <v>33</v>
       </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4">
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36" t="s">
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" t="s">
         <v>35</v>
       </c>
-      <c r="D36" t="s">
-        <v>11</v>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
@@ -1367,133 +1373,157 @@
     </row>
     <row r="38" spans="2:4">
       <c r="B38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>40</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="3:3">
-      <c r="C44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="3:3">
-      <c r="C45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="3:3">
-      <c r="C46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4">
-      <c r="B48" t="s">
-        <v>45</v>
-      </c>
-      <c r="D48" t="s">
-        <v>11</v>
+    <row r="47" spans="3:3">
+      <c r="C47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="3:3">
       <c r="C49" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3">
-      <c r="C50" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="2:4">
-      <c r="B53" t="s">
+    <row r="51" spans="2:4">
+      <c r="B51" t="s">
         <v>49</v>
       </c>
-      <c r="D53" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4">
-      <c r="B54" t="s">
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52" t="s">
         <v>50</v>
       </c>
-      <c r="D54" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4">
-      <c r="B55" t="s">
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53" t="s">
         <v>51</v>
       </c>
-      <c r="D55" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="2:2">
+    <row r="56" spans="2:4">
+      <c r="B56" t="s">
+        <v>53</v>
+      </c>
+      <c r="D56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" t="s">
+        <v>54</v>
+      </c>
+      <c r="D57" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
       <c r="B58" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="59" spans="3:5">
-      <c r="C59" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5">
+      <c r="C62" t="s">
         <v>7</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D62" t="s">
         <v>11</v>
       </c>
-      <c r="E59" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="60" spans="3:5">
-      <c r="C60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="E62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5">
+      <c r="C63" t="s">
+        <v>28</v>
+      </c>
+      <c r="D63" t="s">
         <v>11</v>
       </c>
-      <c r="E60" t="s">
-        <v>55</v>
+      <c r="E63" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>